<commit_message>
day ten first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81789C89-D176-4E59-9C73-CFD2C2550334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A91BE1-99B7-4AA4-85DC-6DB2BF8FD4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions Tracker" sheetId="1" r:id="rId1"/>
+    <sheet name="Concepts to remeber" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Leetcode">'Questions Tracker'!$C$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Topic</t>
   </si>
@@ -79,13 +83,92 @@
   </si>
   <si>
     <t>If number is prime or not</t>
+  </si>
+  <si>
+    <t>1281. Subtract the Product and Sum of Digits of an Integer</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>While loop</t>
+  </si>
+  <si>
+    <t>191. Number of 1 Bits</t>
+  </si>
+  <si>
+    <t>Bitwise Operation</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>number &amp; 1</t>
+  </si>
+  <si>
+    <t>When we do AND of any number with 1 and if it returns 0 then it is an odd number else it is an even number.
+Number&amp;1 - basically does the AND of last bit of that number with 1.</t>
+  </si>
+  <si>
+    <t>Lecture covered</t>
+  </si>
+  <si>
+    <t>Lecture 6: Binary &amp; Decimal Number System</t>
+  </si>
+  <si>
+    <t>answer = (digit * answer^i) + answer</t>
+  </si>
+  <si>
+    <t>answer = (10* answer) + digit</t>
+  </si>
+  <si>
+    <t>Formula to print integer in same flow (ex: 123 -&gt; 123)</t>
+  </si>
+  <si>
+    <t>Formula to reverse an integer (ex: 123 -&gt; 321)</t>
+  </si>
+  <si>
+    <t>Decimal to Binary conversion</t>
+  </si>
+  <si>
+    <t>Integer Range -&gt; (-2^31) to (2^31-1)</t>
+  </si>
+  <si>
+    <t>If you get out of this range it will return garbage value</t>
+  </si>
+  <si>
+    <t>Negative number to binary conversion</t>
+  </si>
+  <si>
+    <t>Program for replacing one digit with other</t>
+  </si>
+  <si>
+    <t>geeksforgeeks</t>
+  </si>
+  <si>
+    <t>Having problem in 2's compliment as how to replace just a single digit in integer so googled it and found this solution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +181,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,10 +232,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -162,8 +254,83 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,22 +643,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DE015C-28F9-428F-8E3F-DA3063A7344F}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" style="13" customWidth="1"/>
     <col min="4" max="4" width="20.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.6328125" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="8" max="8" width="40.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -501,7 +668,7 @@
       <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -527,7 +694,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="3">
         <v>1</v>
       </c>
@@ -551,7 +718,7 @@
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="3">
         <v>1</v>
       </c>
@@ -575,7 +742,7 @@
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="3">
         <v>1</v>
       </c>
@@ -592,8 +759,216 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>44845</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>44845</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>44845</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44876</v>
+      </c>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="32">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28">
+        <v>44876</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{6A12171F-B82B-4AFA-AD02-AF70AA0770D0}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{AF657391-B7C0-4E8D-9015-410D20FF0511}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{28CED1E5-703D-4C1F-A7BA-AD39ABDB401C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97AED2-646B-4C74-8BF8-BADCE88819AE}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" style="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="26"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{CABC0D4D-B593-4D72-96D0-63C398F8EB41}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{FB6ED79F-E1A9-443E-8FEF-AF4A08694CF2}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{5CF1B0B9-27BA-43B2-81CC-AF2E52D28B52}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
eleventh day first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A91BE1-99B7-4AA4-85DC-6DB2BF8FD4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218007D-A4F1-4224-B5DC-FF5C935AD405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Topic</t>
   </si>
@@ -86,18 +86,6 @@
   </si>
   <si>
     <t>1281. Subtract the Product and Sum of Digits of an Integer</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>LeetCode</t>
@@ -137,12 +125,6 @@
     <t>answer = (10* answer) + digit</t>
   </si>
   <si>
-    <t>Formula to print integer in same flow (ex: 123 -&gt; 123)</t>
-  </si>
-  <si>
-    <t>Formula to reverse an integer (ex: 123 -&gt; 321)</t>
-  </si>
-  <si>
     <t>Decimal to Binary conversion</t>
   </si>
   <si>
@@ -162,6 +144,51 @@
   </si>
   <si>
     <t>Having problem in 2's compliment as how to replace just a single digit in integer so googled it and found this solution</t>
+  </si>
+  <si>
+    <t>It basically traverse and go throght number from ones place to tens place then hundredth place and so on. Solve Question 9 to understand</t>
+  </si>
+  <si>
+    <t>Good Question</t>
+  </si>
+  <si>
+    <t>1's complement</t>
+  </si>
+  <si>
+    <t>Flip 0 -&gt; 1 and 1 -&gt; 0</t>
+  </si>
+  <si>
+    <t>2's complement</t>
+  </si>
+  <si>
+    <t>Start from right and move towards left until you find 1, once you find one keep it as it is and flip all the numbers to the left of that 1. That will gove you twos complement of that number.
+Ex: 100100 -&gt; 011100</t>
+  </si>
+  <si>
+    <t>Right Shift</t>
+  </si>
+  <si>
+    <t>Left Shift</t>
+  </si>
+  <si>
+    <t>When we right shift a number, it get divided by 2.
+ex: 4 &gt;&gt; 1 -&gt; In binary 4 is 0100, after one right shift it is 0010 which is nothing but 2, that means 4/2 = 2. so when we do a right shift number gets divided by 2</t>
+  </si>
+  <si>
+    <t>When we left shift a number, it get multiplied by 2.
+ex: 4 &lt;&lt; 1 -&gt; In binary 4 is 0100, after one left shift it is 1000 which is nothing but 8, that means 4*2 = 8. so when we do a left shift number gets multiplied by 2</t>
+  </si>
+  <si>
+    <t>Binary to Decimal Conversion</t>
+  </si>
+  <si>
+    <t>NOTE: is me maine galti kiya ki mai bit level pe solve kr raha tha question. To jb mai 1011 ka AND kiya 1 ke saath to compiler to 1011 ko as a number treat kr raha tha jis ka bit representtion bahot bada tha, to maine seekha ki yaha digit pe work krna hoga. 1011%10 and 1011/10 kr ke solve hoga ye question</t>
+  </si>
+  <si>
+    <t>7. Reverse Integer</t>
+  </si>
+  <si>
+    <t>Formula to print integer in reverse flow (ex: 123 -&gt; 321)</t>
   </si>
 </sst>
 </file>
@@ -194,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,22 +269,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,28 +327,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -643,244 +686,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DE015C-28F9-428F-8E3F-DA3063A7344F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.08984375" customWidth="1"/>
     <col min="2" max="2" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="26.26953125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="12" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.26953125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="20.26953125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="12" style="27" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="29" customWidth="1"/>
     <col min="8" max="8" width="40.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="C2" s="5"/>
+      <c r="D2" s="20">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25">
         <v>44845</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="26">
         <v>0</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="C3" s="5"/>
+      <c r="D3" s="20">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25">
         <v>44845</v>
       </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="5"/>
+      <c r="D4" s="20">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25">
         <v>44845</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="26">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="20">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
         <v>44845</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="26">
         <v>0</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="20">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25">
         <v>44845</v>
       </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="F6" s="26">
+        <v>1</v>
+      </c>
+      <c r="G6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="20">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25">
+        <v>44845</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33">
+        <v>44876</v>
+      </c>
+      <c r="F8" s="34">
+        <v>2</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="9" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="21">
+        <v>1</v>
+      </c>
+      <c r="E9" s="25">
+        <v>44876</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4">
-        <v>44845</v>
-      </c>
-      <c r="F7" s="5">
+    </row>
+    <row r="10" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="20">
+        <v>1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>44906</v>
+      </c>
+      <c r="F10" s="26">
         <v>0</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H10" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1</v>
+      </c>
+      <c r="E11" s="25">
+        <v>44906</v>
+      </c>
+      <c r="F11" s="26">
+        <v>1</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="14">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>44876</v>
-      </c>
-      <c r="F8" s="27">
-        <v>2</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="15" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="32">
-        <v>1</v>
-      </c>
-      <c r="E9" s="28">
-        <v>44876</v>
-      </c>
-      <c r="F9" s="33">
-        <v>0</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -888,87 +979,131 @@
     <hyperlink ref="C5" r:id="rId1" xr:uid="{6A12171F-B82B-4AFA-AD02-AF70AA0770D0}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{AF657391-B7C0-4E8D-9015-410D20FF0511}"/>
     <hyperlink ref="C9" r:id="rId3" xr:uid="{28CED1E5-703D-4C1F-A7BA-AD39ABDB401C}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{EDD6A375-857F-46E5-AB45-B9525BFC3E78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97AED2-646B-4C74-8BF8-BADCE88819AE}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.1796875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="37.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.1796875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" style="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="23" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="B4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="26"/>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CABC0D4D-B593-4D72-96D0-63C398F8EB41}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{FB6ED79F-E1A9-443E-8FEF-AF4A08694CF2}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{5CF1B0B9-27BA-43B2-81CC-AF2E52D28B52}"/>
+    <hyperlink ref="C8" r:id="rId4" display="https://youtu.be/bWrsk0QizEk?list=PLDzeHZWIZsTryvtXdMr6rPh4IDexB5NIA&amp;t=1497" xr:uid="{2A1CECBA-7E00-4D34-A972-E20FD262BAEE}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{AC8AC46C-DBA1-40D0-8FCF-C05ABAB6E128}"/>
+    <hyperlink ref="C8:C9" r:id="rId6" display="Lecture 6: Binary &amp; Decimal Number System" xr:uid="{7483284D-2C95-4B73-92F7-D6B427CFA8F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
second commit of the day
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5218007D-A4F1-4224-B5DC-FF5C935AD405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD07411-3664-412B-9F84-152E849E95A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
     <t>Topic</t>
   </si>
@@ -189,6 +189,26 @@
   </si>
   <si>
     <t>Formula to print integer in reverse flow (ex: 123 -&gt; 321)</t>
+  </si>
+  <si>
+    <t>1009. Complement of Base 10 Integer</t>
+  </si>
+  <si>
+    <t>used masking method and formula of
+(~number) &amp; mask = complement of base 10;</t>
+  </si>
+  <si>
+    <t>(~number)&amp;mask</t>
+  </si>
+  <si>
+    <t>This formula basically flips all the 0's to 1's and vice versa and returns the decimal after that.
+Ex: 8 -&gt; 1000, so after flip 0111 which is 7. So this formula will return 7.</t>
+  </si>
+  <si>
+    <t>231. Power of Two</t>
+  </si>
+  <si>
+    <t>Total Number of setbits in a&amp;b</t>
   </si>
 </sst>
 </file>
@@ -241,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -264,12 +284,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -371,6 +402,13 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,10 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DE015C-28F9-428F-8E3F-DA3063A7344F}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,24 +1013,72 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1</v>
+      </c>
+      <c r="E12" s="25">
+        <v>44906</v>
+      </c>
+      <c r="F12" s="26">
+        <v>2</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="19">
+        <v>1</v>
+      </c>
+      <c r="E13" s="25">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="37" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{6A12171F-B82B-4AFA-AD02-AF70AA0770D0}"/>
     <hyperlink ref="C6" r:id="rId2" xr:uid="{AF657391-B7C0-4E8D-9015-410D20FF0511}"/>
     <hyperlink ref="C9" r:id="rId3" xr:uid="{28CED1E5-703D-4C1F-A7BA-AD39ABDB401C}"/>
     <hyperlink ref="C11" r:id="rId4" xr:uid="{EDD6A375-857F-46E5-AB45-B9525BFC3E78}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{62F2877C-F68E-405C-B8A3-724EDEF538B7}"/>
+    <hyperlink ref="C13" r:id="rId6" xr:uid="{DDEF50B1-D827-4A33-A033-7AC948D5C0D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E97AED2-646B-4C74-8BF8-BADCE88819AE}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,6 +1181,17 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{CABC0D4D-B593-4D72-96D0-63C398F8EB41}"/>
@@ -1102,8 +1200,9 @@
     <hyperlink ref="C8" r:id="rId4" display="https://youtu.be/bWrsk0QizEk?list=PLDzeHZWIZsTryvtXdMr6rPh4IDexB5NIA&amp;t=1497" xr:uid="{2A1CECBA-7E00-4D34-A972-E20FD262BAEE}"/>
     <hyperlink ref="C9" r:id="rId5" xr:uid="{AC8AC46C-DBA1-40D0-8FCF-C05ABAB6E128}"/>
     <hyperlink ref="C8:C9" r:id="rId6" display="Lecture 6: Binary &amp; Decimal Number System" xr:uid="{7483284D-2C95-4B73-92F7-D6B427CFA8F6}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{1DB78E40-65D1-4BCA-89B0-86162280D49D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
twelveth day first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6336A631-AD7D-4602-A574-F67EBD8B2CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7427735-7A6D-4E93-AAC6-FF2DAE6AE47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Topic</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Reverse and array</t>
+  </si>
+  <si>
+    <t>13/11/2022</t>
+  </si>
+  <si>
+    <t>Swap Alternate</t>
   </si>
 </sst>
 </file>
@@ -432,17 +438,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -759,11 +765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40DE015C-28F9-428F-8E3F-DA3063A7344F}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,7 +788,7 @@
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="40" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -880,7 +886,7 @@
       <c r="A5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -956,7 +962,7 @@
       <c r="A8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="31"/>
@@ -1143,16 +1149,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="20"/>
@@ -1219,6 +1225,368 @@
       <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="20"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="20"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="20"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="20"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="20"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="20"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="20"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="20"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="20"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="20"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="20"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="20"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="20"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="20"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="20"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="20"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="20"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="20"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="20"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="20"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="20"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="20"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="20"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="20"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="20"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="20"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="20"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="28"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="20"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="20"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="20"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
last commit for today
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB5B1C7-D3DF-44FA-951E-CB7F438AE3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E25A030-D45A-40E6-94ED-8A3A983C326F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="77">
   <si>
     <t>Topic</t>
   </si>
@@ -262,6 +262,21 @@
   </si>
   <si>
     <t>442. Find All Duplicates in an Array</t>
+  </si>
+  <si>
+    <t>Intersection Of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Pair Sum</t>
+  </si>
+  <si>
+    <t>3Sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not completed </t>
+  </si>
+  <si>
+    <t>Sort 0 1</t>
   </si>
 </sst>
 </file>
@@ -803,8 +818,8 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1381,39 +1396,83 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="19"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="1"/>
+      <c r="B25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="19">
+        <v>1</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="19"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="1"/>
+      <c r="B26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="19">
+        <v>1</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="25">
+        <v>1</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="19"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="25"/>
+      <c r="B27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="19">
+        <v>1</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="25">
+        <v>2</v>
+      </c>
       <c r="G27" s="27"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="19"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="19"/>
+      <c r="D28" s="19">
+        <v>1</v>
+      </c>
       <c r="E28" s="19"/>
       <c r="F28" s="25"/>
       <c r="G28" s="27"/>
@@ -1694,9 +1753,12 @@
     <hyperlink ref="C22" r:id="rId8" xr:uid="{D49C59EA-6145-4221-8FBD-FE0AA1F68CD9}"/>
     <hyperlink ref="C23" r:id="rId9" xr:uid="{63D69603-55B5-4821-A427-D9A8304668F7}"/>
     <hyperlink ref="C24" r:id="rId10" xr:uid="{1B0CF868-B72A-4A70-9C32-4D164D51B07F}"/>
+    <hyperlink ref="C25" r:id="rId11" xr:uid="{91F1A24F-16E0-41DF-BDCA-DD9885716035}"/>
+    <hyperlink ref="C26" r:id="rId12" xr:uid="{2614CDCD-FF3D-41E1-87FB-522C82AE1209}"/>
+    <hyperlink ref="C27" r:id="rId13" xr:uid="{2CCA553C-55B2-430F-8F64-51C76D71C661}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fourteenth day first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F9B4E6-51D1-473D-9497-737DE4DE29A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF56492-08E9-4FEE-9A25-83DA6EE9B2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="91">
   <si>
     <t>Topic</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>852. Peak Index in a Mountain Array</t>
+  </si>
+  <si>
+    <t>Pivot in an Array</t>
+  </si>
+  <si>
+    <t>15/11/2022</t>
   </si>
 </sst>
 </file>
@@ -923,7 +929,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1712,13 +1718,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
-      <c r="B35" s="12"/>
+      <c r="B35" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="1"/>
+      <c r="D35" s="19">
+        <v>1</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="24">
+        <v>2</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="19"/>

</xml_diff>

<commit_message>
first commit sixtheenth day
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28575971-0B26-4692-AD78-23F85506FA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC904A4-2A08-44FC-9C1A-8BB5077E91B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
   <si>
     <t>Topic</t>
   </si>
@@ -337,10 +337,19 @@
     <t>SQRT with precision</t>
   </si>
   <si>
-    <t>15/11.2022</t>
-  </si>
-  <si>
     <t>Allocate Books</t>
+  </si>
+  <si>
+    <t>Painter's Partition Problem</t>
+  </si>
+  <si>
+    <t>16/11/2022</t>
+  </si>
+  <si>
+    <t>Same as book allocation problem</t>
+  </si>
+  <si>
+    <t>Aggressive Cows</t>
   </si>
 </sst>
 </file>
@@ -950,8 +959,8 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1796,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="26" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F37" s="24">
         <v>1</v>
@@ -1816,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F38" s="24">
         <v>1</v>
@@ -1829,7 +1838,7 @@
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="19"/>
       <c r="B39" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>65</v>
@@ -1838,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F39" s="24">
         <v>4</v>
@@ -1850,22 +1859,48 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="19"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="1"/>
+      <c r="B40" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="19">
+        <v>1</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" s="24">
+        <v>4</v>
+      </c>
+      <c r="G40" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="19"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="26"/>
+      <c r="B41" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="19">
+        <v>1</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="24">
+        <v>4</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>13</v>
+      </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -2023,9 +2058,11 @@
     <hyperlink ref="C36" r:id="rId17" xr:uid="{40D06165-76E3-4012-B363-E835CE7CA8F9}"/>
     <hyperlink ref="C37" r:id="rId18" xr:uid="{A18B5A97-4FB9-4F46-BC77-FD667A83A45B}"/>
     <hyperlink ref="C39" r:id="rId19" xr:uid="{9762235F-D464-463C-ABF4-06C1B720F72C}"/>
+    <hyperlink ref="C40" r:id="rId20" xr:uid="{2D2C81B5-1B13-45F9-A833-3151D95C804D}"/>
+    <hyperlink ref="C41" r:id="rId21" xr:uid="{6778B2A9-B4BA-47D1-92FF-474BB9FF05C3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
first commit of the day
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650437D5-3942-474A-816B-6FBC4793A8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951B1B39-F1C4-4DFE-A23B-B0B93A895945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="118">
   <si>
     <t>Topic</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>88. Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>283. Move Zeroes</t>
+  </si>
+  <si>
+    <t>19/11/2022</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1022,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2089,12 +2095,24 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="19"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="26"/>
+      <c r="B48" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="19">
+        <v>1</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="24">
+        <v>1</v>
+      </c>
+      <c r="G48" s="26" t="s">
+        <v>13</v>
+      </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2189,9 +2207,10 @@
     <hyperlink ref="C44" r:id="rId23" xr:uid="{E03520FC-CE99-4597-958B-42471146454F}"/>
     <hyperlink ref="C46" r:id="rId24" xr:uid="{F78F4698-FE61-4CA0-9D59-C973FC8A2A20}"/>
     <hyperlink ref="C47" r:id="rId25" xr:uid="{D2FAC6DE-7BC3-4AB7-9594-0198FBCAF4B2}"/>
+    <hyperlink ref="C48" r:id="rId26" xr:uid="{81577813-0AA5-44F1-97E3-0EF57EB1F430}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ninteenth day first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FFCBF3-9A82-40E9-A711-13191F4F52CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E5706-A14B-4318-8635-09C5CA37F288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="130">
   <si>
     <t>Topic</t>
   </si>
@@ -435,6 +435,18 @@
   </si>
   <si>
     <t>Used the concept that in sorted and roatated array ont one element is greater than the last element.</t>
+  </si>
+  <si>
+    <t>Strings</t>
+  </si>
+  <si>
+    <t>Length of String</t>
+  </si>
+  <si>
+    <t>20/11/2022</t>
+  </si>
+  <si>
+    <t>Reverse of string</t>
   </si>
 </sst>
 </file>
@@ -708,6 +720,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,9 +731,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1039,7 +1051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H52" sqref="H52"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1272,7 +1284,7 @@
       <c r="G9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="50" t="s">
+      <c r="H9" s="47" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1296,7 +1308,7 @@
       <c r="G10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="47" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1419,16 +1431,16 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="50"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="16"/>
@@ -1731,16 +1743,16 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="50"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="16"/>
@@ -1983,16 +1995,16 @@
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="49"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="50"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="16"/>
@@ -2181,28 +2193,44 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" s="16"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="16"/>
+      <c r="A51" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="50"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="16"/>
-      <c r="B52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="C52" s="3"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="16"/>
+      <c r="D52" s="16">
+        <v>1</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F52" s="20">
+        <v>0</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="16" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="16"/>
-      <c r="B53" s="9"/>
+      <c r="B53" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="16"/>
       <c r="E53" s="22"/>
@@ -2221,10 +2249,11 @@
       <c r="H54" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A16:H16"/>
     <mergeCell ref="A30:H30"/>
     <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A51:H51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{6A12171F-B82B-4AFA-AD02-AF70AA0770D0}"/>

</xml_diff>

<commit_message>
twentith day first commit
</commit_message>
<xml_diff>
--- a/All Questions/Question Tracker.xlsx
+++ b/All Questions/Question Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaivishal\Desktop\C++\All Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8936DC-99CD-48EB-8EA2-985F0116DDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8FFB06-9533-4434-9123-9930998C74DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B8276A7-4CE7-41B4-8E94-9ADC3B8771EF}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="137">
   <si>
     <t>Topic</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>Maximum Occuring Character</t>
+  </si>
+  <si>
+    <t>Replace Spaces</t>
+  </si>
+  <si>
+    <t>21/11/2022</t>
   </si>
 </sst>
 </file>
@@ -1066,7 +1072,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2335,12 +2341,24 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="16"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="22"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="22"/>
+      <c r="B57" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="16">
+        <v>1</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="20">
+        <v>0</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>7</v>
+      </c>
       <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -2763,9 +2781,10 @@
     <hyperlink ref="C54" r:id="rId30" xr:uid="{1966F592-02AE-4FBC-89E7-6857BBEA053F}"/>
     <hyperlink ref="C55" r:id="rId31" xr:uid="{9D8BD908-5C46-4C99-B24A-D1FE685B4EDE}"/>
     <hyperlink ref="C56" r:id="rId32" xr:uid="{0D63BBED-553E-4707-97C4-2B5D08BD6A89}"/>
+    <hyperlink ref="C57" r:id="rId33" xr:uid="{8ED1F750-F3FC-4AE8-8C66-046EBF2079FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>